<commit_message>
Section Four Finished - Section Five is about tsconfig.json
</commit_message>
<xml_diff>
--- a/Comandos TypeScript.xlsx
+++ b/Comandos TypeScript.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3C040592-E733-42DB-83BF-3942513EA7DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{79E453B9-4A50-41A2-BC4C-1380421A9924}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Comando</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>Adicionar al tsconfig.json este parametro para que compile por si mismo</t>
+  </si>
+  <si>
+    <t>Parametros de tsconfig.json</t>
+  </si>
+  <si>
+    <t>sourceMap</t>
+  </si>
+  <si>
+    <t>Permite crear un archivo .map para hacer debug en el explorador</t>
   </si>
 </sst>
 </file>
@@ -385,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,6 +470,19 @@
         <v>15</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Section Five finished, most of the changes are in tsconfig.json and xlsx - Section Six is about ES6 new functions and tools
</commit_message>
<xml_diff>
--- a/Comandos TypeScript.xlsx
+++ b/Comandos TypeScript.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{79E453B9-4A50-41A2-BC4C-1380421A9924}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{047716C7-6F2F-4E45-B832-89D5AF3CB0BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Comando</t>
   </si>
@@ -77,16 +77,69 @@
   </si>
   <si>
     <t>Permite crear un archivo .map para hacer debug en el explorador</t>
+  </si>
+  <si>
+    <t>removeComments</t>
+  </si>
+  <si>
+    <t>Tipo boolean</t>
+  </si>
+  <si>
+    <t>Permite indicar si el js se genera con comentarios</t>
+  </si>
+  <si>
+    <t>include</t>
+  </si>
+  <si>
+    <t>Arreglo Strings</t>
+  </si>
+  <si>
+    <t>exclude</t>
+  </si>
+  <si>
+    <t>Permite indicar que directorios incluir en la compilación, no se define dentro del compileroptions</t>
+  </si>
+  <si>
+    <t>Permite indicar que directorios excluir en la compilación, no se define dentro del compileroptions</t>
+  </si>
+  <si>
+    <t>outFile</t>
+  </si>
+  <si>
+    <t>tsc outFile archivoSalida archivo1 archivo2 archivo3</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>http://www.typescriptlang.org/docs/handbook/tsconfig-json.html</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>El parametro file permite indicar los archivos a compilar y esto tambien ayuda a determinar el orden de generación de los archivos en el outfile.</t>
+  </si>
+  <si>
+    <t>en el tsconfig.json recibe la dirección y nombre archivo salida de un compilado de todos los ts files, además se requiere compilar a mano con tsc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,13 +162,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -394,19 +450,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -422,7 +478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -430,7 +486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -438,7 +494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -446,7 +502,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -454,7 +510,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -462,7 +518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -470,20 +526,89 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>18</v>
       </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D17" r:id="rId1" xr:uid="{D108CA36-BDE2-4C4A-9ED7-0FEDAA63FEC9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Section ten finished - Modules With Systems.JS, Modulos.ts/Moduloss.js added, folder Validaciones added, changes in tsconfig.json, index.html now we have package.json because we are working with lite-server
</commit_message>
<xml_diff>
--- a/Comandos TypeScript.xlsx
+++ b/Comandos TypeScript.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{047716C7-6F2F-4E45-B832-89D5AF3CB0BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{409AC6DF-DA20-4D38-AFC3-C1A700D19A63}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Comando</t>
   </si>
@@ -122,6 +122,42 @@
   </si>
   <si>
     <t>en el tsconfig.json recibe la dirección y nombre archivo salida de un compilado de todos los ts files, además se requiere compilar a mano con tsc.</t>
+  </si>
+  <si>
+    <t>Comandos Node</t>
+  </si>
+  <si>
+    <t>npm init</t>
+  </si>
+  <si>
+    <t>Iniciar un proyecto de node.js</t>
+  </si>
+  <si>
+    <t>npm install lite-server --save-dev</t>
+  </si>
+  <si>
+    <t>Instalación de un servidor ligero</t>
+  </si>
+  <si>
+    <t>https://github.com/johnpapa/lite-server</t>
+  </si>
+  <si>
+    <t>npm run dev</t>
+  </si>
+  <si>
+    <t>Ejecuta el servidor configurado</t>
+  </si>
+  <si>
+    <t>npm i npm</t>
+  </si>
+  <si>
+    <t>Instala las dependencias de un proyecto</t>
+  </si>
+  <si>
+    <t>npm install -g lite-server</t>
+  </si>
+  <si>
+    <t>Para instalar globalmente</t>
   </si>
 </sst>
 </file>
@@ -450,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,10 +641,64 @@
         <v>30</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D17" r:id="rId1" xr:uid="{D108CA36-BDE2-4C4A-9ED7-0FEDAA63FEC9}"/>
+    <hyperlink ref="D22" r:id="rId2" xr:uid="{69C1A9DE-570E-4309-A25D-EBD47E63497A}"/>
+    <hyperlink ref="D25" r:id="rId3" xr:uid="{9158C439-147B-4F97-96C5-EEB95783E970}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Section 13 Finished - You will find source to add external libraries and how to add definitions to be used in typescript.
We will find some comments about how to install definitions and how to
use external libraries.
</commit_message>
<xml_diff>
--- a/Comandos TypeScript.xlsx
+++ b/Comandos TypeScript.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{409AC6DF-DA20-4D38-AFC3-C1A700D19A63}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BFFF151A-6E57-41E8-95CC-D27ED9F97E37}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Comando</t>
   </si>
@@ -158,6 +158,28 @@
   </si>
   <si>
     <t>Para instalar globalmente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npm install </t>
+  </si>
+  <si>
+    <t>Instala dependencias de un proyecto</t>
+  </si>
+  <si>
+    <t>npm install --save-dev @types/jquery</t>
+  </si>
+  <si>
+    <t>Instala en la versión de desarrollo un archivo de definición.
+Un archivo de definición contiene todos los elementos que una librería tiene para que typescript no genere error.</t>
+  </si>
+  <si>
+    <t>npm install --save-dev  @types/sweetalert</t>
+  </si>
+  <si>
+    <t>definitelytyped sweetalert</t>
+  </si>
+  <si>
+    <t>termino para buscar la librería de los types a descargar</t>
   </si>
 </sst>
 </file>
@@ -202,9 +224,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -486,15 +511,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -692,13 +717,43 @@
         <v>39</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D17" r:id="rId1" xr:uid="{D108CA36-BDE2-4C4A-9ED7-0FEDAA63FEC9}"/>
     <hyperlink ref="D22" r:id="rId2" xr:uid="{69C1A9DE-570E-4309-A25D-EBD47E63497A}"/>
     <hyperlink ref="D25" r:id="rId3" xr:uid="{9158C439-147B-4F97-96C5-EEB95783E970}"/>
+    <hyperlink ref="A28" r:id="rId4" display="{{{@types/sweetalert" xr:uid="{B71321A3-B6AE-4A59-9FA1-FD018F09C204}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>